<commit_message>
Covariance matrix to CSV file
</commit_message>
<xml_diff>
--- a/cov.xlsx
+++ b/cov.xlsx
@@ -20563,9 +20563,7 @@
       <c r="BQ70" t="n">
         <v>0.001836971318048951</v>
       </c>
-      <c r="BR70" t="n">
-        <v>0.004133293905657103</v>
-      </c>
+      <c r="BR70" t="inlineStr"/>
       <c r="BS70" t="n">
         <v>0.0002912471821399195</v>
       </c>

</xml_diff>